<commit_message>
Added GUI chart feature for Paid vs Pending payments.
</commit_message>
<xml_diff>
--- a/data/payment_records.xlsx
+++ b/data/payment_records.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,6 +478,53 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>avv1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>dee</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D2" t="n">
+        <v>100</v>
+      </c>
+      <c r="E2" t="n">
+        <v>20</v>
+      </c>
+      <c r="F2" t="n">
+        <v>20</v>
+      </c>
+      <c r="G2" t="n">
+        <v>80</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>denememe</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>11.02.2025</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>12.02.2025</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Paid</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>